<commit_message>
parametrize sheet name getter
</commit_message>
<xml_diff>
--- a/tests/testdata/TestBook.xlsx
+++ b/tests/testdata/TestBook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13755"/>
   </bookViews>
   <sheets>
     <sheet name="PolkaDot" sheetId="1" r:id="rId1"/>
@@ -321,6 +321,138 @@
         <a:xfrm>
           <a:off x="4191000" y="1181099"/>
           <a:ext cx="1247775" cy="1247775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="図 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4638675" y="5210174"/>
+          <a:ext cx="1247775" cy="1247775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="図 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="6000750"/>
+          <a:ext cx="1247775" cy="1247775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="図 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5762625" y="476250"/>
+          <a:ext cx="4381500" cy="4381500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2382,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2414,7 +2546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>

</xml_diff>